<commit_message>
feat: update province from config
</commit_message>
<xml_diff>
--- a/data_analysis/config.xlsx
+++ b/data_analysis/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13680"/>
+    <workbookView xWindow="560" yWindow="480" windowWidth="25040" windowHeight="13840"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="273">
   <si>
     <t>A2</t>
   </si>
@@ -872,6 +872,14 @@
   </si>
   <si>
     <t>I2-2-22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>福建省</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scholl_province</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -923,7 +931,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -942,8 +950,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -951,8 +965,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1106,8 +1135,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1117,23 +1170,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="59">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1159,6 +1221,10 @@
     <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1184,6 +1250,10 @@
     <cellStyle name="访问过的超链接" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1488,7 +1558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1496,1319 +1566,1327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B163"/>
+  <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="F146" sqref="F146"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B31" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="8" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B34" s="8" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B35" s="8" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="8" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="8" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="8" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="2" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="24">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:2" ht="24">
+      <c r="A58" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B66" s="7" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B68" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B69" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:2">
+      <c r="A71" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B79" s="7" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="2" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B81" s="7" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="2" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B82" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="7" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="24">
-      <c r="A83" s="2" t="s">
+    <row r="84" spans="1:2" ht="24">
+      <c r="A84" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="7" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="2" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B86" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="2" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B87" s="7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="24">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:2" ht="24">
+      <c r="A88" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:2">
+      <c r="A89" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:2">
+      <c r="A90" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:2">
+      <c r="A91" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="7" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:2">
+      <c r="A92" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:2">
+      <c r="A93" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:2">
+      <c r="A94" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="36">
-      <c r="A95" s="2" t="s">
+    <row r="96" spans="1:2" ht="36">
+      <c r="A96" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:2">
+      <c r="A97" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="2" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="24">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:2" ht="24">
+      <c r="A100" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:2">
+      <c r="A101" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="24">
-      <c r="A101" s="2" t="s">
+    <row r="102" spans="1:2" ht="24">
+      <c r="A102" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B102" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:2">
+      <c r="A103" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B103" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="2" t="s">
+    <row r="104" spans="1:2">
+      <c r="A104" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="2" t="s">
+    <row r="105" spans="1:2">
+      <c r="A105" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B105" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="2" t="s">
+    <row r="106" spans="1:2">
+      <c r="A106" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="2" t="s">
+    <row r="107" spans="1:2">
+      <c r="A107" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B107" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:2">
+      <c r="A108" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B108" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="2" t="s">
+    <row r="109" spans="1:2">
+      <c r="A109" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="2" t="s">
+    <row r="110" spans="1:2">
+      <c r="A110" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B110" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:2">
+      <c r="A111" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B111" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="2" t="s">
+    <row r="112" spans="1:2">
+      <c r="A112" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B112" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="2" t="s">
+    <row r="113" spans="1:2">
+      <c r="A113" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B113" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="2" t="s">
+    <row r="114" spans="1:2">
+      <c r="A114" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:2">
+      <c r="A115" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="2" t="s">
+    <row r="116" spans="1:2">
+      <c r="A116" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B116" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="2" t="s">
+    <row r="117" spans="1:2">
+      <c r="A117" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="2" t="s">
+    <row r="118" spans="1:2">
+      <c r="A118" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B118" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="2" t="s">
+    <row r="119" spans="1:2">
+      <c r="A119" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B119" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="2" t="s">
+    <row r="120" spans="1:2">
+      <c r="A120" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B120" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="2" t="s">
+    <row r="121" spans="1:2">
+      <c r="A121" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="2" t="s">
+    <row r="122" spans="1:2">
+      <c r="A122" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B122" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:2">
+      <c r="A123" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B123" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="2" t="s">
+    <row r="124" spans="1:2">
+      <c r="A124" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B124" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="2" t="s">
+    <row r="125" spans="1:2">
+      <c r="A125" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B125" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="2" t="s">
+    <row r="126" spans="1:2">
+      <c r="A126" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B126" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="2" t="s">
+    <row r="127" spans="1:2">
+      <c r="A127" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B127" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="2" t="s">
+    <row r="128" spans="1:2">
+      <c r="A128" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B128" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="2" t="s">
+    <row r="129" spans="1:2">
+      <c r="A129" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B129" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="2" t="s">
+    <row r="130" spans="1:2">
+      <c r="A130" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B130" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="2" t="s">
+    <row r="131" spans="1:2">
+      <c r="A131" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B131" s="5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="2" t="s">
+    <row r="132" spans="1:2">
+      <c r="A132" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B132" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="2" t="s">
+    <row r="133" spans="1:2">
+      <c r="A133" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B133" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="2" t="s">
+    <row r="134" spans="1:2">
+      <c r="A134" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B134" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="2" t="s">
+    <row r="135" spans="1:2">
+      <c r="A135" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B135" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="2" t="s">
+    <row r="136" spans="1:2">
+      <c r="A136" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B136" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="2" t="s">
+    <row r="137" spans="1:2">
+      <c r="A137" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B137" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
-      <c r="A137" s="2" t="s">
+    <row r="138" spans="1:2">
+      <c r="A138" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B138" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
-      <c r="A138" s="2" t="s">
+    <row r="139" spans="1:2">
+      <c r="A139" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B139" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
-      <c r="A139" s="2" t="s">
+    <row r="140" spans="1:2">
+      <c r="A140" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B140" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
-      <c r="A140" s="2" t="s">
+    <row r="141" spans="1:2">
+      <c r="A141" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B141" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="14" customHeight="1">
-      <c r="A141" s="2" t="s">
+    <row r="142" spans="1:2" ht="14" customHeight="1">
+      <c r="A142" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B142" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="6" t="s">
+    <row r="143" spans="1:2">
+      <c r="A143" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="B142" s="7" t="s">
+      <c r="B143" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
-      <c r="A143" s="6" t="s">
+    <row r="144" spans="1:2">
+      <c r="A144" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="B143" s="7" t="s">
+      <c r="B144" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
-      <c r="A144" s="6" t="s">
+    <row r="145" spans="1:2">
+      <c r="A145" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B144" s="7" t="s">
+      <c r="B145" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="6" t="s">
+    <row r="146" spans="1:2">
+      <c r="A146" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="B145" s="7" t="s">
+      <c r="B146" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="6" t="s">
+    <row r="147" spans="1:2">
+      <c r="A147" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="B146" s="7" t="s">
+      <c r="B147" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="6" t="s">
+    <row r="148" spans="1:2">
+      <c r="A148" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="B147" s="7" t="s">
+      <c r="B148" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="6" t="s">
+    <row r="149" spans="1:2">
+      <c r="A149" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="B148" s="7" t="s">
+      <c r="B149" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="6" t="s">
+    <row r="150" spans="1:2">
+      <c r="A150" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B149" s="7" t="s">
+      <c r="B150" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="6" t="s">
+    <row r="151" spans="1:2">
+      <c r="A151" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="B150" s="7" t="s">
+      <c r="B151" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="6" t="s">
+    <row r="152" spans="1:2">
+      <c r="A152" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="B151" s="7" t="s">
+      <c r="B152" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
-      <c r="A152" s="6" t="s">
+    <row r="153" spans="1:2">
+      <c r="A153" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="B152" s="7" t="s">
+      <c r="B153" s="10" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
-      <c r="A153" s="6" t="s">
+    <row r="154" spans="1:2">
+      <c r="A154" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="B153" s="7" t="s">
+      <c r="B154" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="6" t="s">
+    <row r="155" spans="1:2">
+      <c r="A155" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="B154" s="7" t="s">
+      <c r="B155" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="6" t="s">
+    <row r="156" spans="1:2">
+      <c r="A156" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="B155" s="7" t="s">
+      <c r="B156" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="6" t="s">
+    <row r="157" spans="1:2">
+      <c r="A157" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="B156" s="7" t="s">
+      <c r="B157" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="6" t="s">
+    <row r="158" spans="1:2">
+      <c r="A158" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B157" s="7" t="s">
+      <c r="B158" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
-      <c r="A158" s="6" t="s">
+    <row r="159" spans="1:2">
+      <c r="A159" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B158" s="7" t="s">
+      <c r="B159" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="6" t="s">
+    <row r="160" spans="1:2">
+      <c r="A160" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B159" s="7" t="s">
+      <c r="B160" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="6" t="s">
+    <row r="161" spans="1:2">
+      <c r="A161" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B160" s="7" t="s">
+      <c r="B161" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="6" t="s">
+    <row r="162" spans="1:2">
+      <c r="A162" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B161" s="7" t="s">
+      <c r="B162" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="6" t="s">
+    <row r="163" spans="1:2">
+      <c r="A163" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B162" s="7" t="s">
+      <c r="B163" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="6" t="s">
+    <row r="164" spans="1:2">
+      <c r="A164" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="B163" s="7" t="s">
+      <c r="B164" s="10" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat:add exception when do report
</commit_message>
<xml_diff>
--- a/data_analysis/config.xlsx
+++ b/data_analysis/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="480" windowWidth="25040" windowHeight="13840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -875,11 +875,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>福建省</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>scholl_province</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上海市</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1558,7 +1558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1569,7 +1569,7 @@
   <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1588,10 +1588,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
feat: add emp relative reports
</commit_message>
<xml_diff>
--- a/data_analysis/config.xlsx
+++ b/data_analysis/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="560" yWindow="480" windowWidth="25040" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="276">
   <si>
     <t>A2</t>
   </si>
@@ -880,6 +880,16 @@
   </si>
   <si>
     <t>上海市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一直未就业分布</t>
+  </si>
+  <si>
+    <t>未就业毕业生目前去向分布</t>
+  </si>
+  <si>
+    <t>就业率</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -887,7 +897,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -929,6 +939,11 @@
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF808080"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1160,7 +1175,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1193,6 +1208,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1558,7 +1576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1569,7 +1587,7 @@
   <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1615,7 +1633,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1790,16 +1808,16 @@
       <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>30</v>
+      <c r="B27" s="11" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>30</v>
+      <c r="B28" s="11" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:2">

</xml_diff>

<commit_message>
feat: add job satisfy report
</commit_message>
<xml_diff>
--- a/data_analysis/config.xlsx
+++ b/data_analysis/config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="287">
   <si>
     <t>A2</t>
   </si>
@@ -917,6 +917,15 @@
   </si>
   <si>
     <t>月均收入</t>
+  </si>
+  <si>
+    <t>薪酬满意度</t>
+  </si>
+  <si>
+    <t>职业发展前景</t>
+  </si>
+  <si>
+    <t>工作内容</t>
   </si>
 </sst>
 </file>
@@ -1625,7 +1634,7 @@
   <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1782,24 +1791,24 @@
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>30</v>
+      <c r="B19" s="12" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>30</v>
+      <c r="B20" s="12" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>30</v>
+      <c r="B21" s="12" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:2">

</xml_diff>

<commit_message>
feat: add emp job distribution report
</commit_message>
<xml_diff>
--- a/data_analysis/config.xlsx
+++ b/data_analysis/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="480" windowWidth="25040" windowHeight="13740"/>
+    <workbookView minimized="1" xWindow="560" yWindow="480" windowWidth="25040" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="288">
   <si>
     <t>A2</t>
   </si>
@@ -126,9 +126,6 @@
     <t>职业大类</t>
   </si>
   <si>
-    <t>职业小类</t>
-  </si>
-  <si>
     <t>职业</t>
   </si>
   <si>
@@ -926,6 +923,13 @@
   </si>
   <si>
     <t>工作内容</t>
+  </si>
+  <si>
+    <t>就业行业分布</t>
+  </si>
+  <si>
+    <t>就业职业分布</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1633,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1645,23 +1649,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>31</v>
@@ -1669,7 +1673,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>32</v>
@@ -1680,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1688,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1709,7 +1713,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>31</v>
@@ -1717,7 +1721,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>32</v>
@@ -1725,7 +1729,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>33</v>
@@ -1733,42 +1737,42 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="13">
       <c r="A13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>102</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="13">
+      <c r="A16" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>38</v>
+      <c r="B16" s="13" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="13">
@@ -1776,7 +1780,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1784,7 +1788,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1792,7 +1796,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1800,7 +1804,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1808,7 +1812,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1816,7 +1820,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1824,7 +1828,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="24">
@@ -1832,7 +1836,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1840,7 +1844,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1848,7 +1852,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1856,7 +1860,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1864,7 +1868,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1888,7 +1892,7 @@
         <v>18</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1896,7 +1900,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1904,7 +1908,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1912,7 +1916,7 @@
         <v>21</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1920,7 +1924,7 @@
         <v>22</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1928,7 +1932,7 @@
         <v>23</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1936,7 +1940,7 @@
         <v>24</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1944,23 +1948,23 @@
         <v>25</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1973,578 +1977,578 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="24">
       <c r="A58" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="24">
       <c r="A84" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="24">
       <c r="A88" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="36">
       <c r="A96" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="24">
       <c r="A100" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="24">
       <c r="A102" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2573,7 +2577,7 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>30</v>
@@ -2581,7 +2585,7 @@
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>30</v>
@@ -2589,7 +2593,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>30</v>
@@ -2597,7 +2601,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>30</v>
@@ -2605,354 +2609,354 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="14" customHeight="1">
       <c r="A142" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add emp distribution report
</commit_message>
<xml_diff>
--- a/data_analysis/config.xlsx
+++ b/data_analysis/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="560" yWindow="480" windowWidth="25040" windowHeight="13740"/>
+    <workbookView xWindow="560" yWindow="480" windowWidth="25040" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="292">
   <si>
     <t>A2</t>
   </si>
@@ -930,6 +930,18 @@
   <si>
     <t>就业职业分布</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>就业单位类型</t>
+  </si>
+  <si>
+    <t>就业单位规模</t>
+  </si>
+  <si>
+    <t>就业地区</t>
+  </si>
+  <si>
+    <t>省内就业地区分布</t>
   </si>
 </sst>
 </file>
@@ -1627,7 +1639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1638,7 +1650,7 @@
   <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1699,32 +1711,32 @@
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>30</v>
+      <c r="B7" s="12" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>30</v>
+      <c r="B8" s="11" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>31</v>
+      <c r="B9" s="12" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>32</v>
+      <c r="B10" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>

<commit_message>
feat: add self emp and emp difficult reports
</commit_message>
<xml_diff>
--- a/data_analysis/config.xlsx
+++ b/data_analysis/config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="294">
   <si>
     <t>A2</t>
   </si>
@@ -944,6 +944,14 @@
   </si>
   <si>
     <t>就业单位类型分布</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>求职困难</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>求职成功途径</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1056,8 +1064,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1279,7 +1305,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="65">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1309,6 +1335,9 @@
     <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1338,6 +1367,9 @@
     <cellStyle name="访问过的超链接" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1642,7 +1674,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1652,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1891,7 +1923,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>30</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1899,7 +1931,7 @@
         <v>17</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>30</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:2">

</xml_diff>

<commit_message>
feat: add all reports
</commit_message>
<xml_diff>
--- a/data_analysis/config.xlsx
+++ b/data_analysis/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="0" windowWidth="25040" windowHeight="13780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="299">
   <si>
     <t>A2</t>
   </si>
@@ -965,6 +965,9 @@
   </si>
   <si>
     <t>专业能力</t>
+  </si>
+  <si>
+    <t>对学风认可度评价</t>
   </si>
 </sst>
 </file>
@@ -1705,7 +1708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1715,8 +1718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2650,7 +2653,7 @@
         <v>29</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>30</v>
+        <v>298</v>
       </c>
     </row>
     <row r="117" spans="1:4">

</xml_diff>